<commit_message>
feat: production refresh via GitHub Actions + Google Drive
- .github/workflows/refresh-data.yml: workflow triggered via workflow_dispatch
  - downloads Excel from Google Drive (GDRIVE_FILE_ID secret)
  - runs data_processor.py with Python 3.11
  - commits updated salones_data.json → Vercel auto-redeploys
- api/refresh-data/route.ts: detects VERCEL=1 env var
  - local: runs python3 directly (original behavior unchanged)
  - production: dispatches GitHub Actions workflow via GitHub API (GITHUB_PAT)
- DashboardShell.tsx: new toast UX
  - spinner during loading, disabled state
  - success toast (local, auto-reloads in 800ms)
  - async toast: 'Procesando datos... Vercel actualizará en ~2 min'
  - error toast with message
</commit_message>
<xml_diff>
--- a/app/data/resultados_unificado.xlsx
+++ b/app/data/resultados_unificado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinchapouille/Desktop/Serendip.IA/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1708CF2-14ED-E948-ADDD-DBE391587FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB98541-EE83-6A44-9F8D-609120693F98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13020" yWindow="2300" windowWidth="25380" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1963,9 +1963,9 @@
   </sheetPr>
   <dimension ref="A1:X94"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E43" sqref="E43"/>
+      <selection pane="topRight" activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.83203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
fix: eficiencia backend logic and UI label renames
- data_processor.py Module 3:
  - precio_mt2_ef = costos_fijos / mt2_salon (now covers ALL tiers, not just non-Tier-1)
  - med_pax / med_mt2 computed per tier_salon using precio_mt2_ef
  - desvio_indice_pax = precio_pax / med_pax (exported to JSON)
  - desvio_indice_mt2 = precio_mt2_ef / med_mt2 (exported to JSON)
  - paxRatio and mt2Ratio in JSON now read from precomputed desvio fields
- efficiency/page.tsx:
  - 'Rentabilidad / PAX' renamed to 'Desvío Índice PAX'
  - 'Productividad / m²' renamed to 'Desvío Índice MT2'
  - Descriptions updated: 'precio_x / mediana_x del tier. 1.0 = alineado'
- Regenerated salones_data.json with corrected values
- performance/page.tsx: fixed reference lines (Baja=orange, Media=yellow)
</commit_message>
<xml_diff>
--- a/app/data/resultados_unificado.xlsx
+++ b/app/data/resultados_unificado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinchapouille/Desktop/Serendip.IA/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB98541-EE83-6A44-9F8D-609120693F98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909C841C-468F-E645-892A-0D0EF45FD040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13020" yWindow="2300" windowWidth="25380" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4450,7 +4450,7 @@
         <v>129</v>
       </c>
       <c r="E34" s="2">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>130</v>

</xml_diff>

<commit_message>
fix: use Google Sheets export URL for downloading Excel in workflow
</commit_message>
<xml_diff>
--- a/app/data/resultados_unificado.xlsx
+++ b/app/data/resultados_unificado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinchapouille/Desktop/Serendip.IA/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909C841C-468F-E645-892A-0D0EF45FD040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70D1FCB-343C-5649-8A1A-826E1CD9ABDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13020" yWindow="2300" windowWidth="25380" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1963,9 +1963,9 @@
   </sheetPr>
   <dimension ref="A1:X94"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E35" sqref="E35"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.83203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2627,7 +2627,7 @@
         <v>300</v>
       </c>
       <c r="N9" s="2">
-        <v>1854</v>
+        <v>570</v>
       </c>
       <c r="O9" s="4">
         <v>150</v>
@@ -2701,7 +2701,7 @@
         <v>800</v>
       </c>
       <c r="N10" s="2">
-        <v>570</v>
+        <v>1015</v>
       </c>
       <c r="O10" s="4">
         <v>129</v>
@@ -2775,7 +2775,7 @@
         <v>500</v>
       </c>
       <c r="N11" s="2">
-        <v>1015</v>
+        <v>1105</v>
       </c>
       <c r="O11" s="4">
         <v>112</v>
@@ -2849,7 +2849,7 @@
         <v>500</v>
       </c>
       <c r="N12" s="2">
-        <v>1105</v>
+        <v>1522</v>
       </c>
       <c r="O12" s="4">
         <v>107</v>
@@ -2922,9 +2922,7 @@
       <c r="M13" s="2">
         <v>0</v>
       </c>
-      <c r="N13" s="2">
-        <v>1522</v>
-      </c>
+      <c r="N13" s="2"/>
       <c r="O13" s="4">
         <v>0</v>
       </c>
@@ -2997,7 +2995,7 @@
         <v>200</v>
       </c>
       <c r="N14" s="2">
-        <v>856</v>
+        <v>815</v>
       </c>
       <c r="O14" s="4">
         <v>107</v>
@@ -3071,7 +3069,7 @@
         <v>300</v>
       </c>
       <c r="N15" s="2">
-        <v>815</v>
+        <v>1300</v>
       </c>
       <c r="O15" s="4">
         <v>196</v>
@@ -3145,7 +3143,7 @@
         <v>600</v>
       </c>
       <c r="N16" s="2">
-        <v>1300</v>
+        <v>2674</v>
       </c>
       <c r="O16" s="4">
         <v>66</v>
@@ -3219,7 +3217,7 @@
         <v>180</v>
       </c>
       <c r="N17" s="2">
-        <v>586</v>
+        <v>734</v>
       </c>
       <c r="O17" s="4">
         <v>118</v>
@@ -3293,7 +3291,7 @@
         <v>250</v>
       </c>
       <c r="N18" s="2">
-        <v>2674</v>
+        <v>445</v>
       </c>
       <c r="O18" s="4">
         <v>121</v>
@@ -3367,7 +3365,7 @@
         <v>250</v>
       </c>
       <c r="N19" s="2">
-        <v>734</v>
+        <v>644</v>
       </c>
       <c r="O19" s="4">
         <v>132</v>
@@ -3441,7 +3439,7 @@
         <v>700</v>
       </c>
       <c r="N20" s="2">
-        <v>445</v>
+        <v>340</v>
       </c>
       <c r="O20" s="4">
         <v>89</v>
@@ -3515,7 +3513,7 @@
         <v>250</v>
       </c>
       <c r="N21" s="2">
-        <v>644</v>
+        <v>1683</v>
       </c>
       <c r="O21" s="4">
         <v>78</v>
@@ -3589,7 +3587,7 @@
         <v>150</v>
       </c>
       <c r="N22" s="2">
-        <v>340</v>
+        <v>1457</v>
       </c>
       <c r="O22" s="4">
         <v>93</v>
@@ -3663,7 +3661,7 @@
         <v>800</v>
       </c>
       <c r="N23" s="2">
-        <v>1683</v>
+        <v>1920</v>
       </c>
       <c r="O23" s="4">
         <v>118</v>
@@ -3737,7 +3735,7 @@
         <v>800</v>
       </c>
       <c r="N24" s="2">
-        <v>1457</v>
+        <v>1828</v>
       </c>
       <c r="O24" s="4">
         <v>144</v>
@@ -3811,7 +3809,7 @@
         <v>350</v>
       </c>
       <c r="N25" s="2">
-        <v>1920</v>
+        <v>1056</v>
       </c>
       <c r="O25" s="4">
         <v>130</v>
@@ -3885,7 +3883,7 @@
         <v>550</v>
       </c>
       <c r="N26" s="2">
-        <v>1828</v>
+        <v>429</v>
       </c>
       <c r="O26" s="4">
         <v>128</v>
@@ -3959,7 +3957,7 @@
         <v>180</v>
       </c>
       <c r="N27" s="2">
-        <v>1056</v>
+        <v>1240</v>
       </c>
       <c r="O27" s="4">
         <v>131</v>
@@ -4033,7 +4031,7 @@
         <v>300</v>
       </c>
       <c r="N28" s="2">
-        <v>429</v>
+        <v>607</v>
       </c>
       <c r="O28" s="4">
         <v>80</v>
@@ -4107,7 +4105,7 @@
         <v>500</v>
       </c>
       <c r="N29" s="2">
-        <v>1240</v>
+        <v>5075</v>
       </c>
       <c r="O29" s="4">
         <v>73</v>
@@ -4181,7 +4179,7 @@
         <v>150</v>
       </c>
       <c r="N30" s="2">
-        <v>607</v>
+        <v>2150</v>
       </c>
       <c r="O30" s="4">
         <v>72</v>
@@ -4255,7 +4253,7 @@
         <v>350</v>
       </c>
       <c r="N31" s="2">
-        <v>3185</v>
+        <v>1018</v>
       </c>
       <c r="O31" s="4">
         <v>137</v>
@@ -4328,9 +4326,7 @@
       <c r="M32" s="2">
         <v>0</v>
       </c>
-      <c r="N32" s="2">
-        <v>0</v>
-      </c>
+      <c r="N32" s="2"/>
       <c r="O32" s="4">
         <v>0</v>
       </c>
@@ -4477,7 +4473,7 @@
         <v>200</v>
       </c>
       <c r="N34" s="2">
-        <v>1800</v>
+        <v>1288</v>
       </c>
       <c r="O34" s="4">
         <v>115</v>
@@ -4551,7 +4547,7 @@
         <v>200</v>
       </c>
       <c r="N35" s="2">
-        <v>1331</v>
+        <v>2092</v>
       </c>
       <c r="O35" s="4">
         <v>77</v>
@@ -4625,7 +4621,7 @@
         <v>300</v>
       </c>
       <c r="N36" s="2">
-        <v>1288</v>
+        <v>974</v>
       </c>
       <c r="O36" s="4">
         <v>100</v>
@@ -4699,7 +4695,7 @@
         <v>300</v>
       </c>
       <c r="N37" s="2">
-        <v>2092</v>
+        <v>890</v>
       </c>
       <c r="O37" s="4">
         <v>133</v>
@@ -4773,7 +4769,7 @@
         <v>160</v>
       </c>
       <c r="N38" s="2">
-        <v>974</v>
+        <v>509</v>
       </c>
       <c r="O38" s="4">
         <v>123</v>
@@ -4921,7 +4917,7 @@
         <v>200</v>
       </c>
       <c r="N40" s="2">
-        <v>509</v>
+        <v>1193</v>
       </c>
       <c r="O40" s="4">
         <v>6</v>
@@ -4995,7 +4991,7 @@
         <v>300</v>
       </c>
       <c r="N41" s="2">
-        <v>1193</v>
+        <v>1263</v>
       </c>
       <c r="O41" s="4">
         <v>155</v>
@@ -5069,7 +5065,7 @@
         <v>200</v>
       </c>
       <c r="N42" s="2">
-        <v>1619</v>
+        <v>380</v>
       </c>
       <c r="O42" s="4">
         <v>125</v>
@@ -5143,7 +5139,7 @@
         <v>150</v>
       </c>
       <c r="N43" s="2">
-        <v>380</v>
+        <v>1377</v>
       </c>
       <c r="O43" s="4">
         <v>47</v>
@@ -5217,7 +5213,7 @@
         <v>450</v>
       </c>
       <c r="N44" s="2">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="O44" s="4">
         <v>105</v>
@@ -5291,7 +5287,7 @@
         <v>150</v>
       </c>
       <c r="N45" s="2">
-        <v>1377</v>
+        <v>1277</v>
       </c>
       <c r="O45" s="4">
         <v>128</v>
@@ -5365,7 +5361,7 @@
         <v>450</v>
       </c>
       <c r="N46" s="2">
-        <v>756</v>
+        <v>481</v>
       </c>
       <c r="O46" s="4">
         <v>113</v>
@@ -5439,7 +5435,7 @@
         <v>210</v>
       </c>
       <c r="N47" s="2">
-        <v>1277</v>
+        <v>1008</v>
       </c>
       <c r="O47" s="4">
         <v>131</v>
@@ -5513,7 +5509,7 @@
         <v>200</v>
       </c>
       <c r="N48" s="2">
-        <v>481</v>
+        <v>830</v>
       </c>
       <c r="O48" s="4">
         <v>104</v>
@@ -5587,7 +5583,7 @@
         <v>220</v>
       </c>
       <c r="N49" s="2">
-        <v>1008</v>
+        <v>1345</v>
       </c>
       <c r="O49" s="4">
         <v>130</v>
@@ -5661,7 +5657,7 @@
         <v>250</v>
       </c>
       <c r="N50" s="2">
-        <v>830</v>
+        <v>1500</v>
       </c>
       <c r="O50" s="4">
         <v>111</v>
@@ -5735,7 +5731,7 @@
         <v>270</v>
       </c>
       <c r="N51" s="2">
-        <v>1345</v>
+        <v>1500</v>
       </c>
       <c r="O51" s="4">
         <v>136</v>
@@ -5809,7 +5805,7 @@
         <v>200</v>
       </c>
       <c r="N52" s="2">
-        <v>1500</v>
+        <v>993</v>
       </c>
       <c r="O52" s="4">
         <v>55</v>
@@ -5883,7 +5879,7 @@
         <v>170</v>
       </c>
       <c r="N53" s="2">
-        <v>1500</v>
+        <v>1337</v>
       </c>
       <c r="O53" s="4">
         <v>60</v>
@@ -5957,7 +5953,7 @@
         <v>250</v>
       </c>
       <c r="N54" s="2">
-        <v>16100</v>
+        <v>914</v>
       </c>
       <c r="O54" s="4">
         <v>98</v>
@@ -6031,7 +6027,7 @@
         <v>300</v>
       </c>
       <c r="N55" s="2">
-        <v>993</v>
+        <v>833</v>
       </c>
       <c r="O55" s="4">
         <v>82</v>
@@ -6105,7 +6101,7 @@
         <v>300</v>
       </c>
       <c r="N56" s="2">
-        <v>1337</v>
+        <v>763</v>
       </c>
       <c r="O56" s="4">
         <v>100</v>
@@ -6179,7 +6175,7 @@
         <v>200</v>
       </c>
       <c r="N57" s="2">
-        <v>914</v>
+        <v>1460</v>
       </c>
       <c r="O57" s="4">
         <v>120</v>
@@ -6253,7 +6249,7 @@
         <v>350</v>
       </c>
       <c r="N58" s="2">
-        <v>833</v>
+        <v>650</v>
       </c>
       <c r="O58" s="4">
         <v>89</v>
@@ -6401,7 +6397,7 @@
         <v>300</v>
       </c>
       <c r="N60" s="2">
-        <v>1460</v>
+        <v>570</v>
       </c>
       <c r="O60" s="4">
         <v>85</v>
@@ -6475,7 +6471,7 @@
         <v>400</v>
       </c>
       <c r="N61" s="2">
-        <v>650</v>
+        <v>911</v>
       </c>
       <c r="O61" s="4">
         <v>140</v>
@@ -6623,7 +6619,7 @@
         <v>120</v>
       </c>
       <c r="N63" s="2">
-        <v>911</v>
+        <v>503</v>
       </c>
       <c r="O63" s="4">
         <v>112</v>
@@ -6697,7 +6693,7 @@
         <v>120</v>
       </c>
       <c r="N64" s="2">
-        <v>941</v>
+        <v>730</v>
       </c>
       <c r="O64" s="4">
         <v>94</v>
@@ -6771,7 +6767,7 @@
         <v>100</v>
       </c>
       <c r="N65" s="2">
-        <v>503</v>
+        <v>150</v>
       </c>
       <c r="O65" s="4">
         <v>65</v>
@@ -6845,7 +6841,7 @@
         <v>180</v>
       </c>
       <c r="N66" s="2">
-        <v>730</v>
+        <v>2595</v>
       </c>
       <c r="O66" s="4">
         <v>109</v>
@@ -6919,7 +6915,7 @@
         <v>250</v>
       </c>
       <c r="N67" s="2">
-        <v>270</v>
+        <v>1113</v>
       </c>
       <c r="O67" s="4">
         <v>91</v>
@@ -6993,7 +6989,7 @@
         <v>150</v>
       </c>
       <c r="N68" s="2">
-        <v>150</v>
+        <v>495</v>
       </c>
       <c r="O68" s="4">
         <v>57</v>
@@ -7067,7 +7063,7 @@
         <v>250</v>
       </c>
       <c r="N69" s="2">
-        <v>1113</v>
+        <v>2427</v>
       </c>
       <c r="O69" s="4">
         <v>128</v>
@@ -7141,7 +7137,7 @@
         <v>300</v>
       </c>
       <c r="N70" s="2">
-        <v>495</v>
+        <v>2427</v>
       </c>
       <c r="O70" s="4">
         <v>147</v>
@@ -7215,7 +7211,7 @@
         <v>100</v>
       </c>
       <c r="N71" s="2">
-        <v>2100</v>
+        <v>2427</v>
       </c>
       <c r="O71" s="4">
         <v>88</v>
@@ -7289,7 +7285,7 @@
         <v>200</v>
       </c>
       <c r="N72" s="2">
-        <v>2427</v>
+        <v>1362</v>
       </c>
       <c r="O72" s="4">
         <v>96</v>
@@ -7363,7 +7359,7 @@
         <v>250</v>
       </c>
       <c r="N73" s="2">
-        <v>2427</v>
+        <v>1010</v>
       </c>
       <c r="O73" s="4">
         <v>101</v>
@@ -7437,7 +7433,7 @@
         <v>210</v>
       </c>
       <c r="N74" s="2">
-        <v>2427</v>
+        <v>770</v>
       </c>
       <c r="O74" s="4">
         <v>82</v>
@@ -7511,7 +7507,7 @@
         <v>450</v>
       </c>
       <c r="N75" s="2">
-        <v>1362</v>
+        <v>415</v>
       </c>
       <c r="O75" s="4">
         <v>130</v>
@@ -7585,7 +7581,7 @@
         <v>130</v>
       </c>
       <c r="N76" s="2">
-        <v>1010</v>
+        <v>470</v>
       </c>
       <c r="O76" s="4">
         <v>114</v>
@@ -7659,7 +7655,7 @@
         <v>220</v>
       </c>
       <c r="N77" s="2">
-        <v>770</v>
+        <v>1550</v>
       </c>
       <c r="O77" s="4">
         <v>84</v>
@@ -7733,7 +7729,7 @@
         <v>260</v>
       </c>
       <c r="N78" s="2">
-        <v>415</v>
+        <v>670</v>
       </c>
       <c r="O78" s="4">
         <v>123</v>
@@ -7807,7 +7803,7 @@
         <v>130</v>
       </c>
       <c r="N79" s="2">
-        <v>470</v>
+        <v>500</v>
       </c>
       <c r="O79" s="4">
         <v>122</v>
@@ -7881,7 +7877,7 @@
         <v>200</v>
       </c>
       <c r="N80" s="2">
-        <v>1550</v>
+        <v>1854</v>
       </c>
       <c r="O80" s="4">
         <v>96</v>
@@ -7955,7 +7951,7 @@
         <v>300</v>
       </c>
       <c r="N81" s="2">
-        <v>670</v>
+        <v>586</v>
       </c>
       <c r="O81" s="4">
         <v>94</v>
@@ -8029,7 +8025,7 @@
         <v>250</v>
       </c>
       <c r="N82" s="2">
-        <v>500</v>
+        <v>16100</v>
       </c>
       <c r="O82" s="4">
         <v>90</v>

</xml_diff>